<commit_message>
excel report nuovo aggiornato
</commit_message>
<xml_diff>
--- a/reports/vivado/report-vivado-solutions.xlsx
+++ b/reports/vivado/report-vivado-solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\sintesi-ad-alto-livello-di-sistemi-digitali\progetti\progetto1\reports\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BCC16B-4442-49CA-B36D-C6BFF196AF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99498FAE-D611-4F91-A9A3-854E378ABC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{478786F9-0C08-4B95-A9F2-D12EA5517A72}"/>
   </bookViews>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,22 +328,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -560,6 +557,9 @@
                 <c:pt idx="3">
                   <c:v>1.2505515478551401</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1.32976192981005</c:v>
                 </c:pt>
@@ -725,6 +725,9 @@
                 <c:pt idx="3">
                   <c:v>9.6387171652167994E-2</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54927397286519397</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.38262590533122398</c:v>
                 </c:pt>
@@ -887,6 +890,9 @@
                 <c:pt idx="3">
                   <c:v>0.90053281746804703</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4773420989513399</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.253616715781391</c:v>
                 </c:pt>
@@ -1047,6 +1053,9 @@
                 <c:pt idx="3">
                   <c:v>0.26825189706869401</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56692428188398503</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.92103349743410901</c:v>
                 </c:pt>
@@ -1206,6 +1215,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.260709843132645</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2816495727747701</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.54354930762201503</c:v>
@@ -1368,6 +1380,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>3.1468659926758799E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>4.1766666072362603E-3</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>1.0887121788982801E-2</c:v>
@@ -1532,6 +1547,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.42399298399686802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4121036510914602</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.58537651784718003</c:v>
@@ -1700,6 +1718,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.203573127166238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2914702441739854</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0268509956149519</c:v>
@@ -1848,7 +1869,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2258,7 +2279,7 @@
                   <c:v>3.2035731271662382E-12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.291470244173986E-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2419,7 +2440,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2828,6 +2849,9 @@
                 <c:pt idx="3">
                   <c:v>98</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>384</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>159</c:v>
                 </c:pt>
@@ -2990,6 +3014,9 @@
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3152,6 +3179,9 @@
                 <c:pt idx="3">
                   <c:v>72</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>281</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>147</c:v>
                 </c:pt>
@@ -3312,6 +3342,9 @@
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3470,6 +3503,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -3632,6 +3668,9 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -3796,6 +3835,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -3945,7 +3987,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4354,6 +4396,9 @@
                 <c:pt idx="3">
                   <c:v>57</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>59</c:v>
                 </c:pt>
@@ -4501,7 +4546,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4910,6 +4955,9 @@
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5057,7 +5105,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5466,6 +5514,9 @@
                 <c:pt idx="3">
                   <c:v>4.33</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3519999999999999</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>4.2569999999999997</c:v>
                 </c:pt>
@@ -5613,7 +5664,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -6028,7 +6079,7 @@
                   <c:v>176.3668430335097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>130.75313807531381</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -6189,7 +6240,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -10881,10 +10932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32F8C0C-32ED-409A-A129-79038668F278}">
-  <dimension ref="B2:Z24"/>
+  <dimension ref="B2:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10905,34 +10956,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="O2" s="10" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="O2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="W2" s="10" t="s">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="W2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
     </row>
     <row r="3" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -11016,7 +11067,7 @@
         <f>1000*0.000921480532269925</f>
         <v>0.92148053226992499</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f>1000*3.56509622179146E-06</f>
         <v>3.56509622179146E-3</v>
       </c>
@@ -11082,7 +11133,7 @@
         <f>1000*0.00175678869709373</f>
         <v>1.7567886970937299</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="1">
         <f>1000*0.000414676789660007</f>
         <v>0.41467678966000698</v>
       </c>
@@ -11090,7 +11141,7 @@
         <f>1000*0.000838255044072866</f>
         <v>0.838255044072866</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
         <f>1000*3.34740389007493E-06</f>
         <v>3.3474038900749301E-3</v>
       </c>
@@ -11112,13 +11163,13 @@
       <c r="P6" s="2">
         <v>32</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q6" s="1">
         <v>134</v>
       </c>
       <c r="R6" s="2">
         <v>0</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="1">
         <v>2</v>
       </c>
       <c r="T6" s="2">
@@ -11133,7 +11184,7 @@
       <c r="X6" s="2">
         <v>10</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Y6" s="1">
         <v>3.0739999999999998</v>
       </c>
       <c r="Z6" s="2">
@@ -11156,7 +11207,7 @@
         <f>1000*0.00109893758781254</f>
         <v>1.09893758781254</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="1">
         <f>1000*0.000321194878779352</f>
         <v>0.32119487877935199</v>
       </c>
@@ -11164,7 +11215,7 @@
         <f>1000*0.000590288254898041</f>
         <v>0.59028825489804104</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="1">
         <f>1000*4.16044849771424E-06</f>
         <v>4.1604484977142402E-3</v>
       </c>
@@ -11186,13 +11237,13 @@
       <c r="P7" s="2">
         <v>32</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="1">
         <v>106</v>
       </c>
       <c r="R7" s="2">
         <v>0</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="1">
         <v>2</v>
       </c>
       <c r="T7" s="2">
@@ -11207,7 +11258,7 @@
       <c r="X7" s="2">
         <v>10</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Y7" s="1">
         <v>3.464</v>
       </c>
       <c r="Z7" s="2">
@@ -11231,7 +11282,7 @@
         <f>1000*0.000900532817468047</f>
         <v>0.90053281746804703</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="1">
         <f>1000*0.000268251897068694</f>
         <v>0.26825189706869401</v>
       </c>
@@ -11239,7 +11290,7 @@
         <f>1000*0.000260709843132645</f>
         <v>0.260709843132645</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="1">
         <f>1000*3.14686599267588E-06</f>
         <v>3.1468659926758799E-3</v>
       </c>
@@ -11261,13 +11312,13 @@
       <c r="P8" s="2">
         <v>0</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="Q8" s="1">
         <v>72</v>
       </c>
       <c r="R8" s="2">
         <v>1</v>
       </c>
-      <c r="S8" s="12">
+      <c r="S8" s="1">
         <v>2</v>
       </c>
       <c r="T8" s="2">
@@ -11282,7 +11333,7 @@
       <c r="X8" s="2">
         <v>10</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="Y8" s="1">
         <v>4.33</v>
       </c>
       <c r="Z8" s="2">
@@ -11294,31 +11345,74 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="5"/>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <f>1000*0.000549273972865194</f>
+        <v>0.54927397286519397</v>
+      </c>
+      <c r="F9" s="2">
+        <f>1000*0.00147734209895134</f>
+        <v>1.4773420989513399</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1000*0.000566924281883985</f>
+        <v>0.56692428188398503</v>
+      </c>
+      <c r="H9" s="2">
+        <f>1000*0.00128164957277477</f>
+        <v>1.2816495727747701</v>
+      </c>
+      <c r="I9" s="1">
+        <f>1000*4.17666660723626E-06</f>
+        <v>4.1766666072362603E-3</v>
+      </c>
+      <c r="J9" s="2">
+        <f>1000*0.00141210365109146</f>
+        <v>1.4121036510914602</v>
+      </c>
+      <c r="K9" s="5">
+        <f>SUM(D9:J9)</f>
+        <v>5.2914702441739854</v>
+      </c>
       <c r="M9" s="2">
         <f t="shared" si="0"/>
+        <v>5.291470244173986E-12</v>
+      </c>
+      <c r="O9" s="4">
+        <v>384</v>
+      </c>
+      <c r="P9" s="2">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>281</v>
+      </c>
+      <c r="R9" s="2">
         <v>0</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="5"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="2" t="e">
+      <c r="S9" s="1">
+        <v>2</v>
+      </c>
+      <c r="T9" s="2">
+        <v>71</v>
+      </c>
+      <c r="U9" s="5">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4">
+        <v>39</v>
+      </c>
+      <c r="X9" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="Z9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>130.75313807531381</v>
       </c>
     </row>
     <row r="10" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -11328,9 +11422,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="12"/>
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
       <c r="M10" s="2">
@@ -11339,14 +11431,11 @@
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="12"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="12"/>
       <c r="T10" s="2"/>
       <c r="U10" s="5"/>
       <c r="W10" s="4"/>
       <c r="X10" s="2"/>
-      <c r="Y10" s="12"/>
       <c r="Z10" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -11368,7 +11457,7 @@
         <f>1000*0.000253616715781391</f>
         <v>0.253616715781391</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="1">
         <f>1000*0.000921033497434109</f>
         <v>0.92103349743410901</v>
       </c>
@@ -11376,7 +11465,7 @@
         <f>1000*0.000543549307622015</f>
         <v>0.54354930762201503</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="1">
         <f>1000*0.0000108871217889828</f>
         <v>1.0887121788982801E-2</v>
       </c>
@@ -11398,13 +11487,13 @@
       <c r="P11" s="2">
         <v>0</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="1">
         <v>147</v>
       </c>
       <c r="R11" s="2">
         <v>1</v>
       </c>
-      <c r="S11" s="12">
+      <c r="S11" s="1">
         <v>2</v>
       </c>
       <c r="T11" s="2">
@@ -11419,7 +11508,7 @@
       <c r="X11" s="2">
         <v>10</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="Y11" s="1">
         <v>4.2569999999999997</v>
       </c>
       <c r="Z11" s="2">
@@ -11434,9 +11523,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="12"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="12"/>
       <c r="J12" s="2"/>
       <c r="K12" s="5"/>
       <c r="M12" s="2">
@@ -11445,14 +11532,11 @@
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="12"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="12"/>
       <c r="T12" s="2"/>
       <c r="U12" s="5"/>
       <c r="W12" s="4"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="12"/>
       <c r="Z12" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -11465,9 +11549,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="12"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="12"/>
       <c r="J13" s="2"/>
       <c r="K13" s="5"/>
       <c r="M13" s="2">
@@ -11476,14 +11558,11 @@
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="12"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="12"/>
       <c r="T13" s="2"/>
       <c r="U13" s="5"/>
       <c r="W13" s="4"/>
       <c r="X13" s="2"/>
-      <c r="Y13" s="12"/>
       <c r="Z13" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -11504,7 +11583,7 @@
         <f>1000*0.00121570681221783</f>
         <v>1.2157068122178301</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="1">
         <f>1000*0.000343570427503437</f>
         <v>0.34357042750343703</v>
       </c>
@@ -11512,7 +11591,7 @@
         <f>1000*0.000925468280911446</f>
         <v>0.92546828091144606</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="1">
         <f>1000*3.49782999364834E-06</f>
         <v>3.4978299936483399E-3</v>
       </c>
@@ -11521,7 +11600,7 @@
         <v>1.0144955012947299</v>
       </c>
       <c r="K14" s="5">
-        <f>SUM(D14:J14)</f>
+        <f t="shared" ref="K14:K21" si="2">SUM(D14:J14)</f>
         <v>3.957774796390364</v>
       </c>
       <c r="M14" s="2">
@@ -11534,13 +11613,13 @@
       <c r="P14" s="2">
         <v>32</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="1">
         <v>160</v>
       </c>
       <c r="R14" s="2">
         <v>0</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="1">
         <v>2</v>
       </c>
       <c r="T14" s="2">
@@ -11555,7 +11634,7 @@
       <c r="X14" s="2">
         <v>10</v>
       </c>
-      <c r="Y14" s="12">
+      <c r="Y14" s="1">
         <v>3.6539999999999999</v>
       </c>
       <c r="Z14" s="2">
@@ -11578,7 +11657,7 @@
         <f>1000*0.00160096236504614</f>
         <v>1.60096236504614</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="1">
         <f>1000*0.000303795328363776</f>
         <v>0.30379532836377598</v>
       </c>
@@ -11586,7 +11665,7 @@
         <f>1000*0.000868793693371117</f>
         <v>0.868793693371117</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="1">
         <f>1000*3.56508598997607E-06</f>
         <v>3.5650859899760698E-3</v>
       </c>
@@ -11595,7 +11674,7 @@
         <v>0.85090019274503004</v>
       </c>
       <c r="K15" s="5">
-        <f>SUM(D15:J15)</f>
+        <f t="shared" si="2"/>
         <v>3.9989019692256953</v>
       </c>
       <c r="M15" s="2">
@@ -11608,13 +11687,13 @@
       <c r="P15" s="2">
         <v>32</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="Q15" s="1">
         <v>226</v>
       </c>
       <c r="R15" s="2">
         <v>0</v>
       </c>
-      <c r="S15" s="12">
+      <c r="S15" s="1">
         <v>2</v>
       </c>
       <c r="T15" s="2">
@@ -11629,7 +11708,7 @@
       <c r="X15" s="2">
         <v>9</v>
       </c>
-      <c r="Y15" s="12">
+      <c r="Y15" s="1">
         <v>3.06</v>
       </c>
       <c r="Z15" s="2">
@@ -11652,7 +11731,7 @@
         <f>1000*0.00179032096639276</f>
         <v>1.7903209663927602</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="1">
         <f>1000*0.000363626226317137</f>
         <v>0.36362622631713698</v>
       </c>
@@ -11660,7 +11739,7 @@
         <f>1000*0.00102812109980732</f>
         <v>1.02812109980732</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="1">
         <f>1000*3.38650943376706E-06</f>
         <v>3.3865094337670598E-3</v>
       </c>
@@ -11669,7 +11748,7 @@
         <v>1.07843766454607</v>
       </c>
       <c r="K16" s="5">
-        <f>SUM(D16:J16)</f>
+        <f t="shared" si="2"/>
         <v>4.6963577210590302</v>
       </c>
       <c r="M16" s="2">
@@ -11682,13 +11761,13 @@
       <c r="P16" s="2">
         <v>32</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="1">
         <v>226</v>
       </c>
       <c r="R16" s="2">
         <v>0</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16" s="1">
         <v>2</v>
       </c>
       <c r="T16" s="2">
@@ -11703,7 +11782,7 @@
       <c r="X16" s="2">
         <v>8</v>
       </c>
-      <c r="Y16" s="12">
+      <c r="Y16" s="1">
         <v>2.2770000000000001</v>
       </c>
       <c r="Z16" s="2">
@@ -11726,7 +11805,7 @@
         <f>1000*0.000793763087131083</f>
         <v>0.79376308713108301</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="1">
         <f>1000*0.00162343855481595</f>
         <v>1.62343855481595</v>
       </c>
@@ -11734,7 +11813,7 @@
         <f>1000*0.00104413053486496</f>
         <v>1.0441305348649599</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="1">
         <f>1000*6.84354336044635E-06</f>
         <v>6.8435433604463504E-3</v>
       </c>
@@ -11743,7 +11822,7 @@
         <v>0.78912044409662496</v>
       </c>
       <c r="K17" s="5">
-        <f>SUM(D17:J17)</f>
+        <f t="shared" si="2"/>
         <v>4.9984732863777026</v>
       </c>
       <c r="M17" s="2">
@@ -11756,13 +11835,13 @@
       <c r="P17" s="2">
         <v>32</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="1">
         <v>222</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="1">
         <v>4</v>
       </c>
       <c r="T17" s="2">
@@ -11777,7 +11856,7 @@
       <c r="X17" s="2">
         <v>7</v>
       </c>
-      <c r="Y17" s="12">
+      <c r="Y17" s="1">
         <v>1.33</v>
       </c>
       <c r="Z17" s="2">
@@ -11800,7 +11879,7 @@
         <f>1000*0.000885166635271162</f>
         <v>0.88516663527116202</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="1">
         <f>1000*0.00154896057210863</f>
         <v>1.5489605721086301</v>
       </c>
@@ -11808,7 +11887,7 @@
         <f>1000*0.000758039066568017</f>
         <v>0.75803906656801701</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="1">
         <f>1000*5.97452208239702E-06</f>
         <v>5.9745220823970201E-3</v>
       </c>
@@ -11817,7 +11896,7 @@
         <v>0.69337280001491297</v>
       </c>
       <c r="K18" s="5">
-        <f>SUM(D18:J18)</f>
+        <f t="shared" si="2"/>
         <v>4.5428843882291439</v>
       </c>
       <c r="M18" s="2">
@@ -11830,13 +11909,13 @@
       <c r="P18" s="2">
         <v>32</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="1">
         <v>241</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
       </c>
-      <c r="S18" s="12">
+      <c r="S18" s="1">
         <v>4</v>
       </c>
       <c r="T18" s="2">
@@ -11851,7 +11930,7 @@
       <c r="X18" s="2">
         <v>6</v>
       </c>
-      <c r="Y18" s="12">
+      <c r="Y18" s="1">
         <v>1.573</v>
       </c>
       <c r="Z18" s="2">
@@ -11874,7 +11953,7 @@
         <f>1000*0.00317416270263493</f>
         <v>3.1741627026349302</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="1">
         <f>1000*0.000278797728242353</f>
         <v>0.27879772824235299</v>
       </c>
@@ -11882,7 +11961,7 @@
         <f>1000*0.000888140755705535</f>
         <v>0.88814075570553497</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="1">
         <f>1000*4.53235816166853E-06</f>
         <v>4.5323581616685303E-3</v>
       </c>
@@ -11891,7 +11970,7 @@
         <v>0.85364980623125997</v>
       </c>
       <c r="K19" s="5">
-        <f>SUM(D19:J19)</f>
+        <f t="shared" si="2"/>
         <v>5.756232178555365</v>
       </c>
       <c r="M19" s="2">
@@ -11904,13 +11983,13 @@
       <c r="P19" s="2">
         <v>32</v>
       </c>
-      <c r="Q19" s="12">
+      <c r="Q19" s="1">
         <v>258</v>
       </c>
       <c r="R19" s="2">
         <v>0</v>
       </c>
-      <c r="S19" s="12">
+      <c r="S19" s="1">
         <v>4</v>
       </c>
       <c r="T19" s="2">
@@ -11925,7 +12004,7 @@
       <c r="X19" s="2">
         <v>5</v>
       </c>
-      <c r="Y19" s="12">
+      <c r="Y19" s="1">
         <v>0.374</v>
       </c>
       <c r="Z19" s="2">
@@ -11948,7 +12027,7 @@
         <f>1000*0.00380484666675329</f>
         <v>3.8048466667532899</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="1">
         <f>1000*0.000247060845140368</f>
         <v>0.24706084514036802</v>
       </c>
@@ -11956,7 +12035,7 @@
         <f>1000*0.00072020455263555</f>
         <v>0.72020455263554994</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="1">
         <f>1000*2.47698403654795E-06</f>
         <v>2.4769840365479502E-3</v>
       </c>
@@ -11965,7 +12044,7 @@
         <v>0.68621442187577497</v>
       </c>
       <c r="K20" s="5">
-        <f>SUM(D20:J20)</f>
+        <f t="shared" si="2"/>
         <v>6.032943100535701</v>
       </c>
       <c r="M20" s="2">
@@ -11978,13 +12057,13 @@
       <c r="P20" s="2">
         <v>32</v>
       </c>
-      <c r="Q20" s="12">
+      <c r="Q20" s="1">
         <v>376</v>
       </c>
       <c r="R20" s="2">
         <v>0</v>
       </c>
-      <c r="S20" s="12">
+      <c r="S20" s="1">
         <v>4</v>
       </c>
       <c r="T20" s="2">
@@ -11999,7 +12078,7 @@
       <c r="X20" s="2">
         <v>4</v>
       </c>
-      <c r="Y20" s="12">
+      <c r="Y20" s="1">
         <v>0.45400000000000001</v>
       </c>
       <c r="Z20" s="2">
@@ -12022,7 +12101,7 @@
         <f>1000*0.000642283877823502</f>
         <v>0.64228387782350205</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="1">
         <f>1000*0.00118907087016851</f>
         <v>1.18907087016851</v>
       </c>
@@ -12030,7 +12109,7 @@
         <f>1000*0.00138780823908746</f>
         <v>1.38780823908746</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="1">
         <f>1000*0.000018733164324658</f>
         <v>1.8733164324657998E-2</v>
       </c>
@@ -12039,7 +12118,7 @@
         <v>1.9081661012023701</v>
       </c>
       <c r="K21" s="5">
-        <f>SUM(D21:J21)</f>
+        <f t="shared" si="2"/>
         <v>5.4967950745776779</v>
       </c>
       <c r="M21" s="2">
@@ -12052,13 +12131,13 @@
       <c r="P21" s="2">
         <v>0</v>
       </c>
-      <c r="Q21" s="12">
+      <c r="Q21" s="1">
         <v>458</v>
       </c>
       <c r="R21" s="2">
         <v>0</v>
       </c>
-      <c r="S21" s="12">
+      <c r="S21" s="1">
         <v>2</v>
       </c>
       <c r="T21" s="2">
@@ -12073,7 +12152,7 @@
       <c r="X21" s="2">
         <v>10</v>
       </c>
-      <c r="Y21" s="12">
+      <c r="Y21" s="1">
         <v>4.2080000000000002</v>
       </c>
       <c r="Z21" s="2">
@@ -12090,9 +12169,7 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="12"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="12"/>
       <c r="J22" s="2"/>
       <c r="K22" s="5"/>
       <c r="M22" s="2">
@@ -12101,14 +12178,11 @@
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="12"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="12"/>
       <c r="T22" s="2"/>
       <c r="U22" s="5"/>
       <c r="W22" s="4"/>
       <c r="X22" s="2"/>
-      <c r="Y22" s="12"/>
       <c r="Z22" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -12129,7 +12203,7 @@
         <f>1000*0.00240964675322175</f>
         <v>2.4096467532217498</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="2">
@@ -12158,13 +12232,13 @@
       <c r="P23" s="2">
         <v>0</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="1">
         <v>699</v>
       </c>
       <c r="R23" s="2">
         <v>0</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="1">
         <v>0</v>
       </c>
       <c r="T23" s="2">
@@ -12179,34 +12253,13 @@
       <c r="X23" s="2">
         <v>10</v>
       </c>
-      <c r="Y23" s="12">
+      <c r="Y23" s="1">
         <v>1.369</v>
       </c>
       <c r="Z23" s="2">
         <f t="shared" si="1"/>
         <v>115.86142973004287</v>
       </c>
-    </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
nuovo excel report aggiornato
</commit_message>
<xml_diff>
--- a/reports/vivado/report-vivado-solutions.xlsx
+++ b/reports/vivado/report-vivado-solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\sintesi-ad-alto-livello-di-sistemi-digitali\progetti\progetto1\reports\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649D8122-D786-4298-9479-23690B25A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5102C79-DEFC-4379-B546-5A1D87B1FA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{478786F9-0C08-4B95-A9F2-D12EA5517A72}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Loop Pipelining</t>
+  </si>
+  <si>
+    <t>Solution</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,6 +344,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -560,6 +566,9 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1.32976192981005</c:v>
                 </c:pt>
@@ -588,9 +597,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
@@ -731,6 +737,9 @@
                 <c:pt idx="4">
                   <c:v>0.54927397286519397</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38693009992130101</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.38262590533122398</c:v>
                 </c:pt>
@@ -899,6 +908,9 @@
                 <c:pt idx="4">
                   <c:v>1.4773420989513399</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4364910311996899</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.253616715781391</c:v>
                 </c:pt>
@@ -1065,6 +1077,9 @@
                 <c:pt idx="4">
                   <c:v>0.56692428188398503</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55420439457520798</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.92103349743410901</c:v>
                 </c:pt>
@@ -1230,6 +1245,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.2816495727747701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84493338363245096</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.54354930762201503</c:v>
@@ -1398,6 +1416,9 @@
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>4.1766666072362603E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.3480208660184897E-3</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>1.0887121788982801E-2</c:v>
@@ -1568,6 +1589,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.4121036510914602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98959542810916901</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.58537651784718003</c:v>
@@ -1742,6 +1766,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.2914702441739854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2165023583038366</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0268509956149519</c:v>
@@ -2306,7 +2333,7 @@
                   <c:v>5.291470244173986E-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.2165023583038366E-12</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0268509956149517E-12</c:v>
@@ -2876,6 +2903,9 @@
                 <c:pt idx="4">
                   <c:v>384</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>440</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>159</c:v>
                 </c:pt>
@@ -3044,6 +3074,9 @@
                 <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3212,6 +3245,9 @@
                 <c:pt idx="4">
                   <c:v>281</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>567</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>147</c:v>
                 </c:pt>
@@ -3378,6 +3414,9 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3543,6 +3582,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
@@ -3710,6 +3752,9 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -3880,6 +3925,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -4444,6 +4492,9 @@
                 <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>59</c:v>
                 </c:pt>
@@ -5006,6 +5057,9 @@
                 <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5567,6 +5621,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.3519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1210000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.2569999999999997</c:v>
@@ -6136,7 +6193,7 @@
                   <c:v>130.75313807531381</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>170.09695526450079</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>174.12502176562771</c:v>
@@ -10989,7 +11046,7 @@
   <dimension ref="B2:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11036,7 +11093,10 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:26" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="D3" s="12" t="s">
         <v>32</v>
       </c>
@@ -11473,26 +11533,74 @@
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="5"/>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <f>1000*0.000386930099921301</f>
+        <v>0.38693009992130101</v>
+      </c>
+      <c r="F10" s="2">
+        <f>1000*0.00143649103119969</f>
+        <v>1.4364910311996899</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1000*0.000554204394575208</f>
+        <v>0.55420439457520798</v>
+      </c>
+      <c r="H10" s="2">
+        <f>1000*0.000844933383632451</f>
+        <v>0.84493338363245096</v>
+      </c>
+      <c r="I10" s="1">
+        <f>1000*4.34802086601849E-06</f>
+        <v>4.3480208660184897E-3</v>
+      </c>
+      <c r="J10" s="2">
+        <f>1000*0.000989595428109169</f>
+        <v>0.98959542810916901</v>
+      </c>
+      <c r="K10" s="5">
+        <f>SUM(D10:J10)</f>
+        <v>4.2165023583038366</v>
+      </c>
       <c r="M10" s="2">
         <f t="shared" si="0"/>
+        <v>4.2165023583038366E-12</v>
+      </c>
+      <c r="O10" s="4">
+        <v>440</v>
+      </c>
+      <c r="P10" s="2">
         <v>0</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="5"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="2"/>
-      <c r="Z10" s="2" t="e">
+      <c r="Q10" s="1">
+        <v>567</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>4</v>
+      </c>
+      <c r="T10" s="2">
+        <v>71</v>
+      </c>
+      <c r="U10" s="5">
+        <v>1</v>
+      </c>
+      <c r="W10" s="4">
+        <v>39</v>
+      </c>
+      <c r="X10" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>4.1210000000000004</v>
+      </c>
+      <c r="Z10" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>170.09695526450079</v>
       </c>
     </row>
     <row r="11" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -12266,9 +12374,7 @@
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>

</xml_diff>

<commit_message>
excel report vivado aggiornato
</commit_message>
<xml_diff>
--- a/reports/vivado/report-vivado-solutions.xlsx
+++ b/reports/vivado/report-vivado-solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\sintesi-ad-alto-livello-di-sistemi-digitali\progetti\progetto1\reports\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7403881-33E4-4416-BCF7-3EAA00D9CE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65723EC1-5E5B-40D9-B5FF-98BE7BE0B49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{478786F9-0C08-4B95-A9F2-D12EA5517A72}"/>
   </bookViews>
@@ -558,7 +558,7 @@
                   <c:v>1.2505515478551401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.2408513575792299</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -567,7 +567,7 @@
                   <c:v>1.32976192981005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.23103871010244</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -729,19 +729,19 @@
                   <c:v>9.6387171652167994E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54927397286519397</c:v>
+                  <c:v>8.2524631579872193E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38693009992130101</c:v>
+                  <c:v>0.32527020084671698</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.38262590533122398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67833159118890796</c:v>
+                  <c:v>0.10697833204176301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.57970226043835305</c:v>
+                  <c:v>0.32862459192983801</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.45503594446927298</c:v>
@@ -900,19 +900,19 @@
                   <c:v>0.90053281746804703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4773420989513399</c:v>
+                  <c:v>0.96068286802619696</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4364910311996899</c:v>
+                  <c:v>2.3528356105089201</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.253616715781391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0698106382042201</c:v>
+                  <c:v>0.97222707699984301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5304341688752201</c:v>
+                  <c:v>2.5603906251490098</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.2157068122178301</c:v>
@@ -1069,19 +1069,19 @@
                   <c:v>0.26825189706869401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56692428188398503</c:v>
+                  <c:v>0.27235542074777203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55420439457520798</c:v>
+                  <c:v>0.26371504645794597</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.92103349743410901</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59275847161188699</c:v>
+                  <c:v>0.24706596741452802</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.02545856498182</c:v>
+                  <c:v>0.29804851510562003</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.34357042750343703</c:v>
@@ -1238,19 +1238,19 @@
                   <c:v>0.260709843132645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2816495727747701</c:v>
+                  <c:v>0.26666201301850401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84493338363245096</c:v>
+                  <c:v>0.57519110850989796</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.54354930762201503</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3421794865280401</c:v>
+                  <c:v>0.25889289099723101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4032589970156599</c:v>
+                  <c:v>1.14636321086437</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.92546828091144606</c:v>
@@ -1409,19 +1409,19 @@
                   <c:v>3.1468659926758799E-3</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>4.1766666072362603E-3</c:v>
+                  <c:v>4.2814699554583101E-3</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>4.3480208660184897E-3</c:v>
+                  <c:v>7.01051294527133E-3</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>1.0887121788982801E-2</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>5.8171112868876697E-3</c:v>
+                  <c:v>2.58562499766413E-3</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>5.51955554328742E-3</c:v>
+                  <c:v>3.00649980999879E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.4978299936483399E-3</c:v>
@@ -1582,19 +1582,19 @@
                   <c:v>0.42399298399686802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4121036510914602</c:v>
+                  <c:v>0.42558953282423301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98959542810916901</c:v>
+                  <c:v>0.75069005833938696</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.58537651784718003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.87364441808313</c:v>
+                  <c:v>0.41881192009896001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7241151072084899</c:v>
+                  <c:v>1.32495700381696</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.0144955012947299</c:v>
@@ -1759,19 +1759,19 @@
                   <c:v>3.203573127166238</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2914702441739854</c:v>
+                  <c:v>3.2529472937312667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2165023583038366</c:v>
+                  <c:v>4.2747125376081394</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0268509956149519</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5625417169030733</c:v>
+                  <c:v>3.2376005226524294</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.2684886540628302</c:v>
+                  <c:v>5.6613904466757976</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.957774796390364</c:v>
@@ -2324,19 +2324,19 @@
                   <c:v>3.2035731271662382E-12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.291470244173986E-12</c:v>
+                  <c:v>3.2529472937312669E-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2165023583038366E-12</c:v>
+                  <c:v>4.2747125376081396E-12</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0268509956149517E-12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5625417169030737E-12</c:v>
+                  <c:v>3.2376005226524293E-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.2684886540628295E-12</c:v>
+                  <c:v>5.661390446675798E-12</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.9577747963903639E-12</c:v>
@@ -2889,19 +2889,19 @@
                   <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>384</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>440</c:v>
+                  <c:v>413</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>533</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1016</c:v>
+                  <c:v>1145</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>275</c:v>
@@ -3060,7 +3060,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3069,7 +3069,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3231,19 +3231,19 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>281</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>567</c:v>
+                  <c:v>843</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>452</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>717</c:v>
+                  <c:v>864</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>160</c:v>
@@ -3400,7 +3400,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3409,7 +3409,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3572,7 +3572,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
@@ -3581,7 +3581,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -4478,19 +4478,19 @@
                   <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44</c:v>
@@ -5608,19 +5608,19 @@
                   <c:v>4.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3519999999999999</c:v>
+                  <c:v>4.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1210000000000004</c:v>
+                  <c:v>3.4689999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.2569999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2930000000000001</c:v>
+                  <c:v>4.33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0830000000000002</c:v>
+                  <c:v>3.097</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.6539999999999999</c:v>
@@ -6178,19 +6178,19 @@
                   <c:v>176.3668430335097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130.75313807531381</c:v>
+                  <c:v>176.3668430335097</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170.09695526450079</c:v>
+                  <c:v>153.11590874291838</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>174.12502176562771</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>129.7521733489036</c:v>
+                  <c:v>176.3668430335097</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>126.31047113805735</c:v>
+                  <c:v>144.86455164421264</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>157.5795776867318</c:v>
@@ -11031,7 +11031,7 @@
   <dimension ref="B2:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11445,51 +11445,52 @@
         <v>5</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <f>1000*0.00124085135757923</f>
+        <v>1.2408513575792299</v>
       </c>
       <c r="E9" s="4">
-        <f>1000*0.000549273972865194</f>
-        <v>0.54927397286519397</v>
+        <f>1000*0.0000825246315798722</f>
+        <v>8.2524631579872193E-2</v>
       </c>
       <c r="F9" s="2">
-        <f>1000*0.00147734209895134</f>
-        <v>1.4773420989513399</v>
+        <f>1000*0.000960682868026197</f>
+        <v>0.96068286802619696</v>
       </c>
       <c r="G9" s="1">
-        <f>1000*0.000566924281883985</f>
-        <v>0.56692428188398503</v>
+        <f>1000*0.000272355420747772</f>
+        <v>0.27235542074777203</v>
       </c>
       <c r="H9" s="2">
-        <f>1000*0.00128164957277477</f>
-        <v>1.2816495727747701</v>
+        <f>1000*0.000266662013018504</f>
+        <v>0.26666201301850401</v>
       </c>
       <c r="I9" s="1">
-        <f>1000*4.17666660723626E-06</f>
-        <v>4.1766666072362603E-3</v>
+        <f>1000*4.28146995545831E-06</f>
+        <v>4.2814699554583101E-3</v>
       </c>
       <c r="J9" s="2">
-        <f>1000*0.00141210365109146</f>
-        <v>1.4121036510914602</v>
+        <f>1000*0.000425589532824233</f>
+        <v>0.42558953282423301</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="0"/>
-        <v>5.2914702441739854</v>
+        <f>SUM(D9:J9)</f>
+        <v>3.2529472937312667</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="1"/>
-        <v>5.291470244173986E-12</v>
+        <v>3.2529472937312669E-12</v>
       </c>
       <c r="O9" s="4">
-        <v>384</v>
+        <v>98</v>
       </c>
       <c r="P9" s="2">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1">
-        <v>281</v>
+        <v>72</v>
       </c>
       <c r="R9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="1">
         <v>2</v>
@@ -11501,17 +11502,17 @@
         <v>1</v>
       </c>
       <c r="W9" s="4">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="X9" s="2">
         <v>10</v>
       </c>
       <c r="Y9" s="1">
-        <v>2.3519999999999999</v>
+        <v>4.33</v>
       </c>
       <c r="Z9" s="2">
         <f t="shared" si="2"/>
-        <v>130.75313807531381</v>
+        <v>176.3668430335097</v>
       </c>
     </row>
     <row r="10" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -11522,51 +11523,51 @@
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <f>1000*0.000386930099921301</f>
-        <v>0.38693009992130101</v>
+        <f>1000*0.000325270200846717</f>
+        <v>0.32527020084671698</v>
       </c>
       <c r="F10" s="2">
-        <f>1000*0.00143649103119969</f>
-        <v>1.4364910311996899</v>
+        <f>1000*0.00235283561050892</f>
+        <v>2.3528356105089201</v>
       </c>
       <c r="G10" s="1">
-        <f>1000*0.000554204394575208</f>
-        <v>0.55420439457520798</v>
+        <f>1000*0.000263715046457946</f>
+        <v>0.26371504645794597</v>
       </c>
       <c r="H10" s="2">
-        <f>1000*0.000844933383632451</f>
-        <v>0.84493338363245096</v>
+        <f>1000*0.000575191108509898</f>
+        <v>0.57519110850989796</v>
       </c>
       <c r="I10" s="1">
-        <f>1000*4.34802086601849E-06</f>
-        <v>4.3480208660184897E-3</v>
+        <f>1000*7.01051294527133E-06</f>
+        <v>7.01051294527133E-3</v>
       </c>
       <c r="J10" s="2">
-        <f>1000*0.000989595428109169</f>
-        <v>0.98959542810916901</v>
+        <f>1000*0.000750690058339387</f>
+        <v>0.75069005833938696</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="0"/>
-        <v>4.2165023583038366</v>
+        <f>SUM(D10:J10)</f>
+        <v>4.2747125376081394</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="1"/>
-        <v>4.2165023583038366E-12</v>
+        <v>4.2747125376081396E-12</v>
       </c>
       <c r="O10" s="4">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="P10" s="2">
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>567</v>
+        <v>843</v>
       </c>
       <c r="R10" s="2">
         <v>0</v>
       </c>
       <c r="S10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T10" s="2">
         <v>71</v>
@@ -11575,17 +11576,17 @@
         <v>1</v>
       </c>
       <c r="W10" s="4">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="X10" s="2">
         <v>10</v>
       </c>
       <c r="Y10" s="1">
-        <v>4.1210000000000004</v>
+        <v>3.4689999999999999</v>
       </c>
       <c r="Z10" s="2">
         <f t="shared" si="2"/>
-        <v>170.09695526450079</v>
+        <v>153.11590874291838</v>
       </c>
     </row>
     <row r="11" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -11668,51 +11669,52 @@
         <v>7</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <f>1000*0.00123103871010244</f>
+        <v>1.23103871010244</v>
       </c>
       <c r="E12" s="4">
-        <f>1000*0.000678331591188908</f>
-        <v>0.67833159118890796</v>
+        <f>1000*0.000106978332041763</f>
+        <v>0.10697833204176301</v>
       </c>
       <c r="F12" s="2">
-        <f>1000*0.00206981063820422</f>
-        <v>2.0698106382042201</v>
+        <f>1000*0.000972227076999843</f>
+        <v>0.97222707699984301</v>
       </c>
       <c r="G12" s="1">
-        <f>1000*0.000592758471611887</f>
-        <v>0.59275847161188699</v>
+        <f>1000*0.000247065967414528</f>
+        <v>0.24706596741452802</v>
       </c>
       <c r="H12" s="2">
-        <f>1000*0.00134217948652804</f>
-        <v>1.3421794865280401</v>
+        <f>1000*0.000258892890997231</f>
+        <v>0.25889289099723101</v>
       </c>
       <c r="I12" s="1">
-        <f>1000*5.81711128688767E-06</f>
-        <v>5.8171112868876697E-3</v>
+        <f>1000*2.58562499766413E-06</f>
+        <v>2.58562499766413E-3</v>
       </c>
       <c r="J12" s="2">
-        <f>1000*0.00187364441808313</f>
-        <v>1.87364441808313</v>
+        <f>1000*0.00041881192009896</f>
+        <v>0.41881192009896001</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="0"/>
-        <v>6.5625417169030733</v>
+        <f>SUM(D12:J12)</f>
+        <v>3.2376005226524294</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="1"/>
-        <v>6.5625417169030737E-12</v>
+        <v>3.2376005226524293E-12</v>
       </c>
       <c r="O12" s="4">
-        <v>533</v>
+        <v>145</v>
       </c>
       <c r="P12" s="2">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>452</v>
+        <v>93</v>
       </c>
       <c r="R12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="1">
         <v>2</v>
@@ -11724,17 +11726,17 @@
         <v>1</v>
       </c>
       <c r="W12" s="4">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="X12" s="2">
         <v>10</v>
       </c>
       <c r="Y12" s="1">
-        <v>2.2930000000000001</v>
+        <v>4.33</v>
       </c>
       <c r="Z12" s="2">
         <f t="shared" si="2"/>
-        <v>129.7521733489036</v>
+        <v>176.3668430335097</v>
       </c>
     </row>
     <row r="13" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -11745,51 +11747,51 @@
         <v>0</v>
       </c>
       <c r="E13" s="4">
-        <f>1000*0.000579702260438353</f>
-        <v>0.57970226043835305</v>
+        <f>1000*0.000328624591929838</f>
+        <v>0.32862459192983801</v>
       </c>
       <c r="F13" s="2">
-        <f>1000*0.00253043416887522</f>
-        <v>2.5304341688752201</v>
+        <f>1000*0.00256039062514901</f>
+        <v>2.5603906251490098</v>
       </c>
       <c r="G13" s="1">
-        <f>1000*0.00102545856498182</f>
-        <v>1.02545856498182</v>
+        <f>1000*0.00029804851510562</f>
+        <v>0.29804851510562003</v>
       </c>
       <c r="H13" s="2">
-        <f>1000*0.00140325899701566</f>
-        <v>1.4032589970156599</v>
+        <f>1000*0.00114636321086437</f>
+        <v>1.14636321086437</v>
       </c>
       <c r="I13" s="1">
-        <f>1000*5.51955554328742E-06</f>
-        <v>5.51955554328742E-3</v>
+        <f>1000*3.00649980999879E-06</f>
+        <v>3.00649980999879E-3</v>
       </c>
       <c r="J13" s="2">
-        <f>1000*0.00172411510720849</f>
-        <v>1.7241151072084899</v>
+        <f>1000*0.00132495700381696</f>
+        <v>1.32495700381696</v>
       </c>
       <c r="K13" s="5">
         <f>SUM(D13:J13)</f>
-        <v>7.2684886540628302</v>
+        <v>5.6613904466757976</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="1"/>
-        <v>7.2684886540628295E-12</v>
+        <v>5.661390446675798E-12</v>
       </c>
       <c r="O13" s="4">
-        <v>1016</v>
+        <v>1145</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>717</v>
+        <v>864</v>
       </c>
       <c r="R13" s="2">
         <v>0</v>
       </c>
       <c r="S13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="T13" s="2">
         <v>71</v>
@@ -11798,17 +11800,17 @@
         <v>1</v>
       </c>
       <c r="W13" s="4">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="X13" s="2">
         <v>10</v>
       </c>
       <c r="Y13" s="1">
-        <v>2.0830000000000002</v>
+        <v>3.097</v>
       </c>
       <c r="Z13" s="2">
         <f t="shared" si="2"/>
-        <v>126.31047113805735</v>
+        <v>144.86455164421264</v>
       </c>
     </row>
     <row r="14" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
vivado excel report aggiornato
</commit_message>
<xml_diff>
--- a/reports/vivado/report-vivado-solutions.xlsx
+++ b/reports/vivado/report-vivado-solutions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\sintesi-ad-alto-livello-di-sistemi-digitali\progetti\progetto1\reports\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DAC551-BC5B-4A7B-A95C-C7305080987B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BF5A3-BFB2-436C-8281-F83B4DF87EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" xr2:uid="{478786F9-0C08-4B95-A9F2-D12EA5517A72}"/>
   </bookViews>
@@ -778,7 +778,7 @@
                   <c:v>0.57213963009417101</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.350732821971178</c:v>
+                  <c:v>0.196236724150367</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.36168267251923703</c:v>
@@ -949,7 +949,7 @@
                   <c:v>3.8048466667532899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.64228387782350205</c:v>
+                  <c:v>1.7788336845114798</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.4096467532217498</c:v>
@@ -1118,7 +1118,7 @@
                   <c:v>0.25342355365864899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.18907087016851</c:v>
+                  <c:v>0.81473810132592894</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1287,7 +1287,7 @@
                   <c:v>0.79940224532037996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.38780823908746</c:v>
+                  <c:v>1.27509713638574</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>7.9632550477981603</c:v>
@@ -1458,7 +1458,7 @@
                   <c:v>2.4769840365479502E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>1.8733164324657998E-2</c:v>
+                  <c:v>1.2051522389811E-2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
                   <c:v>8.2827373262262007E-3</c:v>
@@ -1631,7 +1631,7 @@
                   <c:v>0.75632607331499502</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9081661012023701</c:v>
+                  <c:v>1.20656989626586</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5.5387257598340502</c:v>
@@ -1808,7 +1808,7 @@
                   <c:v>6.1886151531780325</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4967950745776779</c:v>
+                  <c:v>5.2835270650291868</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>16.281592970699425</c:v>
@@ -8851,7 +8851,7 @@
                   <c:v>24.75446061271213</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54.967950745776776</c:v>
+                  <c:v>52.835270650291868</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>162.81592970699424</c:v>
@@ -13320,7 +13320,7 @@
                   <c:v>0.45422746916301499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.350732821971178</c:v>
+                  <c:v>0.196236724150367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13395,7 +13395,7 @@
                   <c:v>1.2154849246144299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64228387782350205</c:v>
+                  <c:v>1.7788336845114798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13468,7 +13468,7 @@
                   <c:v>0.33501180587336399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.18907087016851</c:v>
+                  <c:v>0.81473810132592894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13541,7 +13541,7 @@
                   <c:v>0.92148053226992499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.38780823908746</c:v>
+                  <c:v>1.27509713638574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13616,7 +13616,7 @@
                   <c:v>3.56509622179146E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8733164324657998E-2</c:v>
+                  <c:v>1.2051522389811E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13693,7 +13693,7 @@
                   <c:v>1.00705958902836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9081661012023701</c:v>
+                  <c:v>1.20656989626586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13774,7 +13774,7 @@
                   <c:v>3.9368294171708857</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4967950745776779</c:v>
+                  <c:v>5.2835270650291868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14231,7 +14231,7 @@
                   <c:v>39.368294171708854</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.967950745776776</c:v>
+                  <c:v>52.835270650291868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -41180,7 +41180,7 @@
   <dimension ref="B2:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42488,36 +42488,36 @@
         <v>0</v>
       </c>
       <c r="E21" s="4">
-        <f>1000*0.000350732821971178</f>
-        <v>0.350732821971178</v>
+        <f>1000*0.000196236724150367</f>
+        <v>0.196236724150367</v>
       </c>
       <c r="F21" s="2">
-        <f>1000*0.000642283877823502</f>
-        <v>0.64228387782350205</v>
+        <f>1000*0.00177883368451148</f>
+        <v>1.7788336845114798</v>
       </c>
       <c r="G21" s="1">
-        <f>1000*0.00118907087016851</f>
-        <v>1.18907087016851</v>
+        <f>1000*0.000814738101325929</f>
+        <v>0.81473810132592894</v>
       </c>
       <c r="H21" s="2">
-        <f>1000*0.00138780823908746</f>
-        <v>1.38780823908746</v>
+        <f>1000*0.00127509713638574</f>
+        <v>1.27509713638574</v>
       </c>
       <c r="I21" s="1">
-        <f>1000*0.000018733164324658</f>
-        <v>1.8733164324657998E-2</v>
+        <f>1000*0.000012051522389811</f>
+        <v>1.2051522389811E-2</v>
       </c>
       <c r="J21" s="2">
-        <f>1000*0.00190816610120237</f>
-        <v>1.9081661012023701</v>
+        <f>1000*0.00120656989626586</f>
+        <v>1.20656989626586</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" ref="K21" si="4">SUM(D21:J21)</f>
-        <v>5.4967950745776779</v>
+        <v>5.2835270650291868</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="1"/>
-        <v>54.967950745776776</v>
+        <v>52.835270650291868</v>
       </c>
       <c r="O21" s="4">
         <v>311</v>

</xml_diff>